<commit_message>
Backup QR Scanner data - 2025-11-19T10:57:35.769Z - Cache Bust: 1763549855769
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761115032485_d98a641fbd845c0a4e67d5c3df19f56b894b356cbcff263721bcbe66e39d8538.xlsx
+++ b/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761115032485_d98a641fbd845c0a4e67d5c3df19f56b894b356cbcff263721bcbe66e39d8538.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3742,9 +3742,49 @@
         <v>mona.I.hussein@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>244111</v>
+      </c>
+      <c r="B168" t="str">
+        <v>Pathology Lab/Museum</v>
+      </c>
+      <c r="C168" t="str">
+        <v>18/11/2025</v>
+      </c>
+      <c r="D168" t="str">
+        <v>11:11:44</v>
+      </c>
+      <c r="E168" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F168" t="str">
+        <v>mona.I.hussein@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>244055</v>
+      </c>
+      <c r="B169" t="str">
+        <v>Pathology Lab/Museum</v>
+      </c>
+      <c r="C169" t="str">
+        <v>18/11/2025</v>
+      </c>
+      <c r="D169" t="str">
+        <v>11:11:52</v>
+      </c>
+      <c r="E169" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F169" t="str">
+        <v>mona.I.hussein@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F167"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F169"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>